<commit_message>
added draftsman doc to breakout
</commit_message>
<xml_diff>
--- a/Project Outputs for WordStorm Display Breakout PCB/BOM/Bill of Materials-WordStorm Display Breakout PCB.xlsx
+++ b/Project Outputs for WordStorm Display Breakout PCB/BOM/Bill of Materials-WordStorm Display Breakout PCB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\Altium\WordStorm Display Breakout PCB\Project Outputs for WordStorm Display Breakout PCB\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4AAF5A47-0B49-4D1E-BF95-600A3B1EDD01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7D1C4DDA-BC0A-4DF6-A216-392AEE363EE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="1485" windowWidth="21600" windowHeight="13065" xr2:uid="{8300F5AF-32C2-411E-8BF4-F9A04E7E4D54}"/>
+    <workbookView xWindow="4800" yWindow="1485" windowWidth="21600" windowHeight="13065" xr2:uid="{A56AA6F8-7013-4C84-9704-29AA60102FA1}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-WordStorm Dis" sheetId="1" r:id="rId1"/>
@@ -464,7 +464,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4673591-EB3B-4E90-B506-F94324F477E2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97317FEE-5F48-41A3-BAB9-7B2169BC4DD5}">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>